<commit_message>
update EAMT - Planilha Abrelpe
</commit_message>
<xml_diff>
--- a/1 etim ds 2022/EAMT/Planilha Abrelpe RSU.xlsx
+++ b/1 etim ds 2022/EAMT/Planilha Abrelpe RSU.xlsx
@@ -1,24 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1 etim ds 2022\EAMT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{489DDC18-463A-4CC1-8A98-2A82FE136BC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9CE6E55-ED10-4554-B3D0-0A16669BEA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{78BE9437-7E1D-4B2D-BC9F-1BCAD08AE796}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -33,34 +43,34 @@
     <t>Regiões</t>
   </si>
   <si>
+    <t>Ano</t>
+  </si>
+  <si>
     <t>Norte</t>
   </si>
   <si>
+    <t>4,406,280</t>
+  </si>
+  <si>
     <t>Nordeste</t>
   </si>
   <si>
+    <t>17,397,725</t>
+  </si>
+  <si>
     <t>Centro-Oeste</t>
   </si>
   <si>
-    <t>Ano</t>
+    <t>5,076,055</t>
   </si>
   <si>
     <t>Sudeste</t>
   </si>
   <si>
+    <t>32,652,900</t>
+  </si>
+  <si>
     <t>Sul</t>
-  </si>
-  <si>
-    <t>4,406,280</t>
-  </si>
-  <si>
-    <t>17,397,725</t>
-  </si>
-  <si>
-    <t>5,076,055</t>
-  </si>
-  <si>
-    <t>32,652,900</t>
   </si>
   <si>
     <t>7,162,760</t>
@@ -72,9 +82,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,14 +93,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -157,9 +159,6 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -167,24 +166,27 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -237,7 +239,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -539,31 +541,32 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="10"/>
       <c r="B3">
         <v>2010</v>
       </c>
@@ -571,45 +574,59 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="11">
+        <v>5866645</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="11">
+        <v>19700875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="12"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="C6" s="12">
+        <v>5815180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="12">
+        <v>39442995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
+      </c>
+      <c r="C8" s="11">
+        <v>8243890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update EAMT - Planilhas atualizadas | LPL
</commit_message>
<xml_diff>
--- a/1 etim ds 2022/EAMT/Planilha Abrelpe RSU.xlsx
+++ b/1 etim ds 2022/EAMT/Planilha Abrelpe RSU.xlsx
@@ -1,41 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1 etim ds 2022\EAMT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1 etim ds 2022\EAMT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9CE6E55-ED10-4554-B3D0-0A16669BEA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5C90B9-0D5D-4A5C-92E1-9358AFF07A7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{78BE9437-7E1D-4B2D-BC9F-1BCAD08AE796}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{78BE9437-7E1D-4B2D-BC9F-1BCAD08AE796}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>Geração Absoluta Total (T/Ano)</t>
   </si>
@@ -84,7 +74,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,15 +167,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -239,7 +229,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -535,38 +525,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98AC5662-B49A-4B7A-9BE5-005F9A4F4A49}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="10"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
       <c r="B3">
         <v>2010</v>
       </c>
@@ -574,66 +564,198 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <v>5866645</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>19700875</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <v>5815180</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="10">
         <v>39442995</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>8243890</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="11"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13">
+        <v>2010</v>
+      </c>
+      <c r="C13">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23">
+        <v>2010</v>
+      </c>
+      <c r="C23">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="9">
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>